<commit_message>
Iniciando o r markdown
</commit_message>
<xml_diff>
--- a/DocenteConsulta.xlsx
+++ b/DocenteConsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorB\Desktop\ArquivosPesquisaUNB\Rpibic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7DA712-987C-4144-8409-7BE443F84B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C3311C-0E04-486F-BE70-5E6427D644C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2286,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DI1" workbookViewId="0">
-      <selection activeCell="DS9" sqref="DS9"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
+      <selection activeCell="BT6" sqref="BT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,7 +3463,7 @@
         <v>113</v>
       </c>
       <c r="BS6" s="2"/>
-      <c r="BT6" s="2" t="s">
+      <c r="BT6" s="4" t="s">
         <v>122</v>
       </c>
       <c r="BV6" s="2"/>

</xml_diff>

<commit_message>
Arrumado tabelas dos alunos
</commit_message>
<xml_diff>
--- a/DocenteConsulta.xlsx
+++ b/DocenteConsulta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorB\Desktop\ArquivosPesquisaUNB\Rpibic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34573CAC-12DB-4148-A0DA-E296EAB3B902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB60658-50D4-4352-B027-799C32EBA520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2290,8 +2290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>